<commit_message>
inmplemnting condition for edit code groupe
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C42459
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Zone</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Codes</t>
+  </si>
+  <si>
+    <t>Services</t>
   </si>
 </sst>
 </file>
@@ -402,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +449,7 @@
     <col min="3" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,6 +467,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rate change type column
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C43557
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wissam.ajamy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\TOneV2\Code\TOneV2\TOne.WhS.BusinessEntity.Web\WhS_BusinessEntity\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Zone</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Zone-Fix</t>
+  </si>
+  <si>
+    <t>Change Type</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -63,7 +69,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000;[Red]0.0000"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -93,7 +99,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,19 +108,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9958800012207406E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,23 +131,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,86 +422,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="6">
         <v>36550</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="5">
         <v>0.9</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="6">
         <v>36550</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Increment filed to template
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C44267
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/Sale Pricelist Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Zone</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Rate EED</t>
   </si>
   <si>
-    <t>CLIENT</t>
-  </si>
-  <si>
     <t>Codes</t>
   </si>
   <si>
@@ -61,6 +58,15 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>CLIENT Logo &amp; Info</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -439,12 +445,13 @@
     <col min="7" max="7" width="15.7109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -454,13 +461,14 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -478,18 +486,21 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="6">
         <v>36550</v>
@@ -501,15 +512,18 @@
         <v>36550</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>